<commit_message>
Updated VIN Upload files to match the changes made in the scope of PAS-2715
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/VINupload_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/VINupload_CA_CHOICE.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>VIN</t>
   </si>
@@ -101,18 +101,12 @@
     <t>ANTITHEFTCODE_TEXT</t>
   </si>
   <si>
-    <t>STAT</t>
-  </si>
-  <si>
     <t>COLL_SYMBOL</t>
   </si>
   <si>
     <t>COMP_SYMBOL</t>
   </si>
   <si>
-    <t>CHOICE_TIER</t>
-  </si>
-  <si>
     <t>ALTFUEL</t>
   </si>
   <si>
@@ -164,17 +158,41 @@
     <t>BBBKN3DD&amp;E</t>
   </si>
   <si>
-    <t>Cargo Van</t>
-  </si>
-  <si>
-    <t>I</t>
+    <t>BI_SYMBOL</t>
+  </si>
+  <si>
+    <t>PD_SYMBOL</t>
+  </si>
+  <si>
+    <t>UM_SYMBOL</t>
+  </si>
+  <si>
+    <t>MP_SYMBOL</t>
+  </si>
+  <si>
+    <t>ENTRYDATE</t>
+  </si>
+  <si>
+    <t>VALID</t>
+  </si>
+  <si>
+    <t>ANTITHEFT_DISCOUNT</t>
+  </si>
+  <si>
+    <t>RESTRAINTS_DISCOUNT</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,8 +214,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +232,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -219,20 +249,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -511,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AJ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AI12" sqref="AI12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,13 +563,14 @@
     <col min="23" max="23" width="22.21875" customWidth="1"/>
     <col min="24" max="24" width="20.88671875" customWidth="1"/>
     <col min="25" max="25" width="34.77734375" customWidth="1"/>
-    <col min="26" max="26" width="22.77734375" customWidth="1"/>
-    <col min="27" max="27" width="14.88671875" customWidth="1"/>
-    <col min="28" max="28" width="16.21875" customWidth="1"/>
-    <col min="29" max="29" width="17" customWidth="1"/>
+    <col min="26" max="26" width="14.88671875" customWidth="1"/>
+    <col min="27" max="27" width="16.21875" customWidth="1"/>
+    <col min="33" max="33" width="15.109375" customWidth="1"/>
+    <col min="35" max="35" width="22.6640625" customWidth="1"/>
+    <col min="36" max="36" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,106 +655,142 @@
       <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
+      <c r="AC1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C2" s="3">
         <v>2017</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H2" s="3">
         <v>53080</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O2" s="3">
         <v>8</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="3">
         <v>214</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="S2" s="3">
         <v>2</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="V2" s="3">
         <v>2</v>
       </c>
       <c r="W2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="X2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3">
         <v>39</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="AA2" s="3">
         <v>39</v>
       </c>
-      <c r="AB2" s="3">
-        <v>39</v>
+      <c r="AB2" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>40</v>
+        <v>52</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG2">
+        <v>20000101</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -748,8 +818,6 @@
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>